<commit_message>
Adding coloured branches based on Class
</commit_message>
<xml_diff>
--- a/data/Data_extraction_postcrosschecking.xlsx
+++ b/data/Data_extraction_postcrosschecking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z3439723_ad_unsw_edu_au/Documents/Overview of reviews_trans environment effects/Analysis/Nongen_map_of_reviews/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="551" documentId="8_{5C8DE252-67D3-437E-999F-0322730C74C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{266BCD83-1113-4D2F-93BD-6AAE9990697D}"/>
+  <xr:revisionPtr revIDLastSave="552" documentId="8_{5C8DE252-67D3-437E-999F-0322730C74C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7584C4ED-54D4-4265-9F0C-C836A4364D10}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E4D07577-1050-462D-A7B0-049CD472D6CE}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6081" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6082" uniqueCount="1182">
   <si>
     <t>id</t>
   </si>
@@ -3651,6 +3651,9 @@
   </si>
   <si>
     <t>Hexanauplia</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
@@ -16478,8 +16481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61DB050-FA39-425C-8BE9-84756207D428}">
   <dimension ref="A1:D559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
-      <selection activeCell="H552" sqref="H552"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16497,6 +16500,9 @@
       </c>
       <c r="C1" t="s">
         <v>277</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1181</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>